<commit_message>
add external dns service test case
</commit_message>
<xml_diff>
--- a/alibaba_clound_dns_testcase.xlsx
+++ b/alibaba_clound_dns_testcase.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tracyho/Desktop/rancher/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tracyho/Desktop/rancher/rancher-test_case/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="3620" yWindow="1160" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="alibaba cloud dns" sheetId="1" r:id="rId1"/>
-    <sheet name="工作表2" sheetId="2" r:id="rId2"/>
+    <sheet name="one host" sheetId="1" r:id="rId1"/>
+    <sheet name="two hosts" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="57">
   <si>
     <t>module</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -70,10 +70,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>rancher catalog -alibaba cloud dns test case</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>launch</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -110,10 +106,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>fail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>v0.1.1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -166,35 +158,66 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>alidns catalog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>special character</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>version</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DNS Name Template</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>preview</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017/8/30 下午9:58:26time="2017-08-30T13:58:26Z" level=error msg="Failed to update provider with new DNS records: Provider error reading dns entries: Alibaba Cloud API call has failed: Aliyun API Error: RequestId:  Status Code: -1 Code: AliyunGoClientFailure Message: json: cannot unmarshal string into Go struct field RecordType.TTL of type int32"</t>
+  </si>
+  <si>
+    <t>launch workpress before alidns launch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>particular number</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>alidns catalog</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>special character</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>pass</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>version</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DNS Name Template</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>default value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>preview</t>
+    <t>launch workpress after alidns launch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete workpress on rancher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete workpress on aliyun</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -206,14 +229,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>sync up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>host switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete one of the host</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>pass</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2017/8/30 下午9:58:26time="2017-08-30T13:58:26Z" level=error msg="Failed to update provider with new DNS records: Provider error reading dns entries: Alibaba Cloud API call has failed: Aliyun API Error: RequestId:  Status Code: -1 Code: AliyunGoClientFailure Message: json: cannot unmarshal string into Go struct field RecordType.TTL of type int32"</t>
-  </si>
-  <si>
-    <t>particular number</t>
+    <t>add one more host</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -221,38 +253,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>delete workpress</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>delete alidns</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dns service</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>launch workpress after alidns launch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>launch workpress before alidns launch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a host</t>
-  </si>
-  <si>
-    <t>two hosts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a host</t>
+    <t>alidns service  exit before</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -292,7 +293,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,12 +309,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,10 +414,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -451,8 +442,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -731,11 +728,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0.25"/>
@@ -786,13 +783,13 @@
     </row>
     <row r="2" spans="1:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>38</v>
-      </c>
       <c r="C2" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
@@ -800,14 +797,14 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="22"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -815,13 +812,13 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="20" t="s">
-        <v>23</v>
+      <c r="B4" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="C4" s="6" t="b">
         <v>1</v>
@@ -832,12 +829,12 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="21"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="6" t="b">
         <v>0</v>
       </c>
@@ -847,14 +844,14 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="21"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -862,13 +859,13 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="20" t="s">
-        <v>24</v>
+      <c r="B7" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="C7" s="6" t="b">
         <v>1</v>
@@ -879,12 +876,12 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="21"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="6" t="b">
         <v>0</v>
       </c>
@@ -894,14 +891,14 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="21"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -909,13 +906,13 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="20" t="s">
-        <v>26</v>
+      <c r="B10" s="18" t="s">
+        <v>24</v>
       </c>
       <c r="C10" s="6" t="b">
         <v>1</v>
@@ -926,12 +923,12 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="21"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="6" t="b">
         <v>0</v>
       </c>
@@ -941,14 +938,14 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="21"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -956,14 +953,14 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="21"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -971,14 +968,14 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="21"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -986,14 +983,14 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="21"/>
-      <c r="C15" s="18" t="s">
-        <v>46</v>
+      <c r="B15" s="19"/>
+      <c r="C15" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1001,27 +998,27 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="21"/>
-      <c r="C16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="2:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="22"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1029,16 +1026,16 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="2:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="20" t="s">
-        <v>39</v>
+      <c r="B18" s="18" t="s">
+        <v>36</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -1046,12 +1043,12 @@
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="2:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="21"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="6" t="b">
         <v>0</v>
       </c>
@@ -1061,14 +1058,14 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="2:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="21"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -1076,14 +1073,14 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="21"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -1091,14 +1088,14 @@
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="2:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="21"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -1106,14 +1103,14 @@
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="2:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="21"/>
-      <c r="C23" s="18" t="s">
-        <v>34</v>
+      <c r="B23" s="19"/>
+      <c r="C23" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -1121,27 +1118,27 @@
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J23" s="8"/>
     </row>
     <row r="24" spans="2:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="21"/>
-      <c r="C24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="2:10" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="22"/>
+      <c r="B25" s="20"/>
       <c r="C25" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -1149,137 +1146,115 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="2:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="H26" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="22"/>
+      <c r="C27" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="24"/>
-      <c r="C27" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="10" t="s">
+      <c r="I27" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="23"/>
+      <c r="C28" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H28" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I27" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="25"/>
-      <c r="C28" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>18</v>
-      </c>
       <c r="I28" s="14" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="2:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="2:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="I30" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J30" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="I31" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J30" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="14" t="s">
+    </row>
+    <row r="32" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="25"/>
+      <c r="C32" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="25"/>
+      <c r="C33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="26"/>
+      <c r="C34" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="I31" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="15"/>
-      <c r="C32" s="14" t="s">
+      <c r="I34" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="I32" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="17"/>
-      <c r="C33" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="I33" s="16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="I34" s="14" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="35" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="I35" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="I36" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="17"/>
-      <c r="C37" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="I37" s="14" t="s">
-        <v>51</v>
-      </c>
+      <c r="B35" s="15"/>
+    </row>
+    <row r="36" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="B31:B34"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="B18:B25"/>
     <mergeCell ref="B26:B28"/>
@@ -1296,29 +1271,162 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="33.5" style="13" customWidth="1"/>
+    <col min="3" max="3" width="38.83203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="21" style="5" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="5"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="25"/>
+      <c r="C3" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="25"/>
+      <c r="C4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="26"/>
+      <c r="C5" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="C6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="22"/>
+      <c r="C7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+      <c r="C8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="15"/>
+      <c r="C10" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>